<commit_message>
Se agrega el proyecto
</commit_message>
<xml_diff>
--- a/Datos.xlsx
+++ b/Datos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SemilleroSQA\coronaScreenplay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F26A10-ED47-4E3F-922C-69FFEA2C21B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CC363A-8722-4B03-B116-1D2B89B17435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7875" xr2:uid="{3540448D-15D3-497D-A489-A650C2B94990}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3540448D-15D3-497D-A489-A650C2B94990}"/>
   </bookViews>
   <sheets>
     <sheet name="DatosRegistro" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
     <t>pineda</t>
   </si>
   <si>
-    <t>7@gmail.com</t>
+    <t>12@gmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>